<commit_message>
Corrigida função que salva a rede. Iniciados testes com a base MNIST. Todo: criar função para salvar população, para poder parar o treinamento e continuar depois.
</commit_message>
<xml_diff>
--- a/Xor_Genetic.xlsx
+++ b/Xor_Genetic.xlsx
@@ -38,7 +38,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -64,6 +64,13 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
     <border>
@@ -447,7 +454,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,10 +472,12 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="n"/>
-      <c r="D1" s="1" t="n">
+      <c r="D1" s="1" t="n"/>
+      <c r="E1" s="1" t="n"/>
+      <c r="F1" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="n"/>
+      <c r="G1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -483,9 +492,15 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E2" s="1" t="n">
+      <c r="G2" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -494,16 +509,22 @@
         <v>0</v>
       </c>
       <c r="B4" t="n">
-        <v>4.307709026009078</v>
+        <v>3.995910303355823</v>
       </c>
       <c r="C4" t="n">
-        <v>-12.04447704155604</v>
+        <v>-9.595948218959755</v>
       </c>
       <c r="D4" t="n">
-        <v>8.26792402307002</v>
+        <v>-9.824522234801375</v>
       </c>
       <c r="E4" t="n">
-        <v>-14.85089138709381</v>
+        <v>3.012523386384068</v>
+      </c>
+      <c r="F4" t="n">
+        <v>16.94989531332135</v>
+      </c>
+      <c r="G4" t="n">
+        <v>-17.37845937967623</v>
       </c>
     </row>
     <row r="5">
@@ -511,16 +532,22 @@
         <v>1</v>
       </c>
       <c r="B5" t="n">
-        <v>3.767339116572964</v>
+        <v>2.0499316506778</v>
       </c>
       <c r="C5" t="n">
-        <v>-11.667391693184</v>
+        <v>-4.492484374931386</v>
       </c>
       <c r="D5" t="n">
-        <v>9.064465412192149</v>
+        <v>-5.290784327382515</v>
       </c>
       <c r="E5" t="n">
-        <v>-12.80714756008984</v>
+        <v>8.555680557054506</v>
+      </c>
+      <c r="F5" t="n">
+        <v>6.542476586241063</v>
+      </c>
+      <c r="G5" t="n">
+        <v>-3.536985016217162</v>
       </c>
     </row>
     <row r="6">
@@ -528,22 +555,58 @@
         <v>2</v>
       </c>
       <c r="B6" t="n">
-        <v>-2</v>
+        <v>-3.721699685396691</v>
       </c>
       <c r="C6" t="n">
-        <v>-6</v>
+        <v>-5.811602190161497</v>
       </c>
       <c r="D6" t="n">
-        <v>6</v>
+        <v>-5.21462714713974</v>
       </c>
       <c r="E6" t="n">
-        <v>-5</v>
+        <v>0.0397458734780809</v>
+      </c>
+      <c r="F6" t="n">
+        <v>9.501351289512513</v>
+      </c>
+      <c r="G6" t="n">
+        <v>-17.68165301722782</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="n">
+        <v>2.7888057487887</v>
+      </c>
+      <c r="G7" t="n">
+        <v>-8.389815711943996</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="n">
+        <v>7.135461618165352</v>
+      </c>
+      <c r="G8" t="n">
+        <v>-10.14564680090852</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:G1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -608,7 +671,7 @@
       </c>
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D3" t="n">
         <v>0.9</v>

</xml_diff>

<commit_message>
Iniciada integração com scikit learn
</commit_message>
<xml_diff>
--- a/Xor_Genetic.xlsx
+++ b/Xor_Genetic.xlsx
@@ -509,22 +509,22 @@
         <v>0</v>
       </c>
       <c r="B4" t="n">
-        <v>3.995910303355823</v>
+        <v>-0.1937348010753318</v>
       </c>
       <c r="C4" t="n">
-        <v>-9.595948218959755</v>
+        <v>-6.785386184910475</v>
       </c>
       <c r="D4" t="n">
-        <v>-9.824522234801375</v>
+        <v>1.689551354844047</v>
       </c>
       <c r="E4" t="n">
-        <v>3.012523386384068</v>
+        <v>-6.297125354620201</v>
       </c>
       <c r="F4" t="n">
-        <v>16.94989531332135</v>
+        <v>7.403454951011472</v>
       </c>
       <c r="G4" t="n">
-        <v>-17.37845937967623</v>
+        <v>-12.85121242792387</v>
       </c>
     </row>
     <row r="5">
@@ -532,22 +532,22 @@
         <v>1</v>
       </c>
       <c r="B5" t="n">
-        <v>2.0499316506778</v>
+        <v>4.990699365056803</v>
       </c>
       <c r="C5" t="n">
-        <v>-4.492484374931386</v>
+        <v>-8.508136534546692</v>
       </c>
       <c r="D5" t="n">
-        <v>-5.290784327382515</v>
+        <v>-2.207094393071722</v>
       </c>
       <c r="E5" t="n">
-        <v>8.555680557054506</v>
+        <v>5.407402955309999</v>
       </c>
       <c r="F5" t="n">
-        <v>6.542476586241063</v>
+        <v>10.36228188534344</v>
       </c>
       <c r="G5" t="n">
-        <v>-3.536985016217162</v>
+        <v>-12.99689402641534</v>
       </c>
     </row>
     <row r="6">
@@ -555,22 +555,22 @@
         <v>2</v>
       </c>
       <c r="B6" t="n">
-        <v>-3.721699685396691</v>
+        <v>-0.4726016765291365</v>
       </c>
       <c r="C6" t="n">
-        <v>-5.811602190161497</v>
+        <v>-4.016155106674934</v>
       </c>
       <c r="D6" t="n">
-        <v>-5.21462714713974</v>
+        <v>1.427217109486305</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0397458734780809</v>
+        <v>-0.722224203175398</v>
       </c>
       <c r="F6" t="n">
-        <v>9.501351289512513</v>
+        <v>9.189570846447866</v>
       </c>
       <c r="G6" t="n">
-        <v>-17.68165301722782</v>
+        <v>-9.780724066055841</v>
       </c>
     </row>
     <row r="7">
@@ -582,10 +582,10 @@
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="n">
-        <v>2.7888057487887</v>
+        <v>-2.741007145283092</v>
       </c>
       <c r="G7" t="n">
-        <v>-8.389815711943996</v>
+        <v>6.18552779297814</v>
       </c>
     </row>
     <row r="8">
@@ -597,10 +597,10 @@
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="n">
-        <v>7.135461618165352</v>
+        <v>3.04798120154035</v>
       </c>
       <c r="G8" t="n">
-        <v>-10.14564680090852</v>
+        <v>-3.785340261565299</v>
       </c>
     </row>
   </sheetData>

</xml_diff>